<commit_message>
Moved the process to a method
</commit_message>
<xml_diff>
--- a/ExcelDrivenData.xlsx
+++ b/ExcelDrivenData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Self improvement\Selenium Udemy\Code\ExcelDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983D7DAB-F9FB-4A6F-A06E-71B9EE3B480C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2007A8A1-FA1C-4CB6-BE31-A491B5632DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{4F54D588-5BEA-4932-AD00-8346E5BA4186}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Testcases</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>Anik4</t>
+  </si>
+  <si>
+    <t>A123</t>
+  </si>
+  <si>
+    <t>A124</t>
+  </si>
+  <si>
+    <t>A125</t>
+  </si>
+  <si>
+    <t>A126</t>
   </si>
 </sst>
 </file>
@@ -437,7 +449,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,8 +478,8 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
-        <v>123</v>
+      <c r="D2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -480,8 +492,8 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3">
-        <v>124</v>
+      <c r="D3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -494,8 +506,8 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4">
-        <v>125</v>
+      <c r="D4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -508,8 +520,8 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5">
-        <v>126</v>
+      <c r="D5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the ability to handle numerical cell values.
Using NumberToTextConverter
</commit_message>
<xml_diff>
--- a/ExcelDrivenData.xlsx
+++ b/ExcelDrivenData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Self improvement\Selenium Udemy\Code\ExcelDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2007A8A1-FA1C-4CB6-BE31-A491B5632DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B639BF-34B5-4C90-B091-2613B82B8697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="2280" windowWidth="21600" windowHeight="11385" xr2:uid="{4F54D588-5BEA-4932-AD00-8346E5BA4186}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Testcases</t>
   </si>
@@ -77,18 +77,6 @@
   </si>
   <si>
     <t>Anik4</t>
-  </si>
-  <si>
-    <t>A123</t>
-  </si>
-  <si>
-    <t>A124</t>
-  </si>
-  <si>
-    <t>A125</t>
-  </si>
-  <si>
-    <t>A126</t>
   </si>
 </sst>
 </file>
@@ -449,7 +437,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,8 +466,8 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
+      <c r="D2">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -492,8 +480,8 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
+      <c r="D3">
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -506,8 +494,8 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
+      <c r="D4">
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -520,8 +508,8 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>17</v>
+      <c r="D5">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>